<commit_message>
Added RMS test script
</commit_message>
<xml_diff>
--- a/DataFiles/excel/Login/LoginDetails.xlsx
+++ b/DataFiles/excel/Login/LoginDetails.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="6" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23901"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\HardDiskCopied\E\InelliJ\SeleniumTestJavaArtifact2july\SeleniumTestJavaArtifact\DataFiles\excel\Login\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{71DA45F1-FB98-463D-BC75-5D60FA52A54B}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="-105" windowWidth="19425" windowHeight="10425"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Valid_Login" sheetId="3" r:id="rId1"/>
@@ -12,22 +18,16 @@
     <sheet name="ConsignmentID" sheetId="4" r:id="rId3"/>
   </sheets>
   <calcPr calcId="124519"/>
-  <extLst xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main">
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+  <extLst>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="26">
   <si>
     <t>RunToTest</t>
   </si>
@@ -77,21 +77,6 @@
     <t>Passed</t>
   </si>
   <si>
-    <t>opensourcecms</t>
-  </si>
-  <si>
-    <t>demo1</t>
-  </si>
-  <si>
-    <t>6P06xCcG478a4(UeLbVblG5s</t>
-  </si>
-  <si>
-    <t>brnwinjit@gmail.com</t>
-  </si>
-  <si>
-    <t>Winjit@123</t>
-  </si>
-  <si>
     <t>surekha.jadhav@ram.co.za</t>
   </si>
   <si>
@@ -113,20 +98,20 @@
     <t>anand.maurya@ram.co.za</t>
   </si>
   <si>
-    <t>Surekha@003</t>
-  </si>
-  <si>
     <t>Nasreen.khan@ram.co.za</t>
   </si>
   <si>
     <t>Nasreen@123</t>
+  </si>
+  <si>
+    <t>Surekha@123123</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -440,29 +425,29 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E8"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="9.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="46.28515625" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="39.140625" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="57.140625" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="9.5546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="46.33203125" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="39.109375" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="57.109375" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -479,114 +464,68 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:5">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>16</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>7</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5">
+        <v>22</v>
+      </c>
+      <c r="C3" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>7</v>
       </c>
-      <c r="B4" t="s">
-        <v>17</v>
-      </c>
-      <c r="C4" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5">
-      <c r="A5" t="s">
-        <v>7</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5">
-      <c r="A6" t="s">
-        <v>7</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5">
-      <c r="A7" t="s">
-        <v>7</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="C7" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5">
-      <c r="A8" t="s">
-        <v>3</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="C8" s="1" t="s">
-        <v>30</v>
+      <c r="B4" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>24</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B5" r:id="rId1"/>
-    <hyperlink ref="C5" r:id="rId2"/>
-    <hyperlink ref="B6" r:id="rId3"/>
-    <hyperlink ref="B7" r:id="rId4"/>
-    <hyperlink ref="C6" r:id="rId5"/>
-    <hyperlink ref="B8" r:id="rId6"/>
-    <hyperlink ref="C8" r:id="rId7"/>
+    <hyperlink ref="B2" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
+    <hyperlink ref="B3" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
+    <hyperlink ref="C2" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
+    <hyperlink ref="B4" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
+    <hyperlink ref="C4" r:id="rId5" xr:uid="{00000000-0004-0000-0000-000006000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="9.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="26.5703125" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="13.42578125" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="57.140625" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="9.5546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="26.5546875" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="13.44140625" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="57.109375" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -603,7 +542,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:5">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -617,7 +556,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="3" spans="1:5">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>7</v>
       </c>
@@ -628,7 +567,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:5">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>7</v>
       </c>
@@ -639,7 +578,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:5">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>7</v>
       </c>
@@ -655,49 +594,49 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B2" r:id="rId1"/>
-    <hyperlink ref="B3" r:id="rId2"/>
-    <hyperlink ref="B4" r:id="rId3"/>
-    <hyperlink ref="B5" r:id="rId4"/>
+    <hyperlink ref="B2" r:id="rId1" xr:uid="{00000000-0004-0000-0100-000000000000}"/>
+    <hyperlink ref="B3" r:id="rId2" xr:uid="{00000000-0004-0000-0100-000001000000}"/>
+    <hyperlink ref="B4" r:id="rId3" xr:uid="{00000000-0004-0000-0100-000002000000}"/>
+    <hyperlink ref="B5" r:id="rId4" xr:uid="{00000000-0004-0000-0100-000003000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="9.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="20.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.5546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="20.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="C1" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>3</v>
       </c>
       <c r="B2" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="C2" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
27 Feb-Added Script for external user profile
</commit_message>
<xml_diff>
--- a/DataFiles/excel/Login/LoginDetails.xlsx
+++ b/DataFiles/excel/Login/LoginDetails.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23901"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26026"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\HardDiskCopied\E\InelliJ\SeleniumTestJavaArtifact2july\SeleniumTestJavaArtifact\DataFiles\excel\Login\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Nasreen\HardDiskCopied\E\InelliJ\SeleniumTestJavaArtifact2july\SeleniumTestJavaArtifact\DataFiles\excel\Login\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{71DA45F1-FB98-463D-BC75-5D60FA52A54B}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F520C407-E928-49A4-B238-9E411BFD83CB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="27">
   <si>
     <t>RunToTest</t>
   </si>
@@ -105,6 +105,9 @@
   </si>
   <si>
     <t>Surekha@123123</t>
+  </si>
+  <si>
+    <t>Nasreenk@winjit.com</t>
   </si>
 </sst>
 </file>
@@ -433,10 +436,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E4"/>
+  <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -466,7 +469,7 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>16</v>
@@ -495,6 +498,17 @@
       </c>
       <c r="C4" s="1" t="s">
         <v>24</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>26</v>
       </c>
     </row>
   </sheetData>
@@ -504,6 +518,8 @@
     <hyperlink ref="C2" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
     <hyperlink ref="B4" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
     <hyperlink ref="C4" r:id="rId5" xr:uid="{00000000-0004-0000-0000-000006000000}"/>
+    <hyperlink ref="B5" r:id="rId6" xr:uid="{EF5C0708-49C4-48DD-9EF0-D54D5C5D3787}"/>
+    <hyperlink ref="C5" r:id="rId7" xr:uid="{AF3D40E2-552A-4432-8BC1-E28899F9AD13}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>